<commit_message>
added some research data
</commit_message>
<xml_diff>
--- a/public/budget_data.xlsx
+++ b/public/budget_data.xlsx
@@ -331,7 +331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3110" uniqueCount="441">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="512">
   <si>
     <t>-</t>
   </si>
@@ -1662,6 +1662,219 @@
   </si>
   <si>
     <t>Depayment of Defence PBS</t>
+  </si>
+  <si>
+    <t>Families &amp; Children</t>
+  </si>
+  <si>
+    <t>Family Support</t>
+  </si>
+  <si>
+    <t>Parent and Baby Payments</t>
+  </si>
+  <si>
+    <t>Family Tax Benefit</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Housing Assistance and Homelessness Prevention</t>
+  </si>
+  <si>
+    <t>Affordable Housing</t>
+  </si>
+  <si>
+    <t>Community Capability and the Vulnerable</t>
+  </si>
+  <si>
+    <t>Financial Management</t>
+  </si>
+  <si>
+    <t>Community Investment</t>
+  </si>
+  <si>
+    <t>Income Support for Vulnerable People</t>
+  </si>
+  <si>
+    <t>Support for People in Special Circumstances</t>
+  </si>
+  <si>
+    <t>To improve the financial knowledge, skills, capabilities and financial  resilience of vulnerable individuals and families to alleviate the immediate impact of financial stress, and to progress initiatives in relation to problem gambling.</t>
+  </si>
+  <si>
+    <t>Supplementary Payments and Support for Income Support Recipients</t>
+  </si>
+  <si>
+    <t>Seniors</t>
+  </si>
+  <si>
+    <t>Income Support for Seniors</t>
+  </si>
+  <si>
+    <t>Allow ances, Concessions and Services for seniors</t>
+  </si>
+  <si>
+    <t>Disability and Carers</t>
+  </si>
+  <si>
+    <t>Targeted Community Care</t>
+  </si>
+  <si>
+    <t>Disability Support Pension</t>
+  </si>
+  <si>
+    <t>Income Support for Carers</t>
+  </si>
+  <si>
+    <t>Support for Carers</t>
+  </si>
+  <si>
+    <t>National Disability Insurance Scheme</t>
+  </si>
+  <si>
+    <t>Early Intervention Services for Children with Disability</t>
+  </si>
+  <si>
+    <t>Services and Support for People with Disability</t>
+  </si>
+  <si>
+    <t>Women</t>
+  </si>
+  <si>
+    <t>To implement strategies in priority areas to achieve gender equality. The priority areas include reducing violence against women, improving economic outcomes for women, and ensuring women’s equal place in society</t>
+  </si>
+  <si>
+    <t>Indigenous</t>
+  </si>
+  <si>
+    <t>Economic Development and Participation</t>
+  </si>
+  <si>
+    <t>Indigenous Housing and Infrastructure</t>
+  </si>
+  <si>
+    <t>Indigenous Capability and Development</t>
+  </si>
+  <si>
+    <t>Stronger Futures in the Northern Territory</t>
+  </si>
+  <si>
+    <t>Native Title and Land Rights</t>
+  </si>
+  <si>
+    <t>Aboriginal Hostels Limited</t>
+  </si>
+  <si>
+    <t>Families, Housing, Community Services and indigenous affairs portfolio</t>
+  </si>
+  <si>
+    <t>Department of Families, Housing, Community Services and indigenous affairs</t>
+  </si>
+  <si>
+    <t>Community Operated Hostels</t>
+  </si>
+  <si>
+    <t>Company Operated Hostels</t>
+  </si>
+  <si>
+    <t>Australian Institute of Family Studies</t>
+  </si>
+  <si>
+    <t>Equal Opportunity for Women in the workplace</t>
+  </si>
+  <si>
+    <t>Indigenous Business Australia</t>
+  </si>
+  <si>
+    <t>Equities and Investments</t>
+  </si>
+  <si>
+    <t>Business Development and Assistance</t>
+  </si>
+  <si>
+    <t>Indigenous Home Ownership</t>
+  </si>
+  <si>
+    <t>Indigenous Land Corporation</t>
+  </si>
+  <si>
+    <t>Torres Strait Regional Authority</t>
+  </si>
+  <si>
+    <t>http://resources.fahcsia.gov.au/budget/2012-13/FaHCSIA_PBS_2012-13.pdf</t>
+  </si>
+  <si>
+    <t>Families, Housing, Community Services and Indigenous Affairs Portfolio Budget Statement</t>
+  </si>
+  <si>
+    <t>Data not yet collected</t>
+  </si>
+  <si>
+    <t>Industry Innovation, Science, Research &amp; Tertiary Education Portfolio</t>
+  </si>
+  <si>
+    <t>Department of Industry, Innovation, Science, Research and Tertiary Education</t>
+  </si>
+  <si>
+    <t>Australian industry support</t>
+  </si>
+  <si>
+    <t>Industry Development and Investment</t>
+  </si>
+  <si>
+    <t>Program Support</t>
+  </si>
+  <si>
+    <t>Innovative Industry</t>
+  </si>
+  <si>
+    <t>Automotive Transformation Scheme</t>
+  </si>
+  <si>
+    <t>Clean Technol ogy Investment</t>
+  </si>
+  <si>
+    <t>Liquefied Petroleum Gas Vehicle Scheme</t>
+  </si>
+  <si>
+    <t>Cooperati ve Resear ch Centres Program</t>
+  </si>
+  <si>
+    <t>Green Car Innovation Fund</t>
+  </si>
+  <si>
+    <t>Commercialisation Australia</t>
+  </si>
+  <si>
+    <t>Science &amp; Research</t>
+  </si>
+  <si>
+    <t>Investment in Higher Education Research</t>
+  </si>
+  <si>
+    <t>Science &amp;  Research Capacity</t>
+  </si>
+  <si>
+    <t>Joint Research Engagement Program</t>
+  </si>
+  <si>
+    <t>International Postgraduate Research Scholarship Scheme</t>
+  </si>
+  <si>
+    <t>Research Infrastructure Block Grants</t>
+  </si>
+  <si>
+    <t>Research Training Scheme</t>
+  </si>
+  <si>
+    <t>Sustainable Research Excellence in Universities</t>
+  </si>
+  <si>
+    <t>The Australian Postgraduate Awards</t>
+  </si>
+  <si>
+    <t>The Commercialisation Training Scheme</t>
   </si>
 </sst>
 </file>
@@ -1763,7 +1976,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="543">
+  <cellStyleXfs count="645">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2307,8 +2520,110 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2329,9 +2644,10 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="543">
+  <cellStyles count="645">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2603,6 +2919,57 @@
     <cellStyle name="Followed Hyperlink" xfId="538" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="540" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="542" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="544" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="546" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="548" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="550" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="552" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="554" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="556" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="558" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="560" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="562" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="564" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="566" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="568" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="570" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="572" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="574" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="576" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="578" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="580" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="582" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="584" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="586" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="588" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="590" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="592" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="594" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="596" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="598" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="600" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="602" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="604" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="606" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="608" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="610" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="612" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="614" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="616" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="618" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="620" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="622" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="624" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="626" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="628" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="630" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="632" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="634" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="636" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="638" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2874,6 +3241,57 @@
     <cellStyle name="Hyperlink" xfId="537" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="539" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="541" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="543" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="545" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="547" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="549" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="551" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="553" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="555" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="557" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="559" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="561" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="563" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="565" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="567" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="569" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="571" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="573" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="575" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="577" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="579" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="581" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="583" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="585" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="587" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="589" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="591" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="593" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="595" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="597" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="599" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="601" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="603" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="605" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="607" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="609" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="611" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="613" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="615" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="617" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="619" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="621" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="623" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="625" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="627" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="629" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="631" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="633" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="635" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="637" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3256,7 +3674,7 @@
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:12">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>220</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -3277,21 +3695,21 @@
       <c r="G3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="15" t="s">
         <v>32</v>
       </c>
       <c r="J3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="14"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
@@ -3310,12 +3728,12 @@
       <c r="G4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
       <c r="J4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="14"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
@@ -4200,10 +4618,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U291"/>
+  <dimension ref="A1:U346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B238" workbookViewId="0">
-      <selection activeCell="F280" sqref="F280"/>
+    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="B338" sqref="B338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11028,201 +11446,1431 @@
     </row>
     <row r="274" spans="1:10">
       <c r="A274" t="s">
-        <v>388</v>
-      </c>
-      <c r="F274" s="1">
-        <f>365800000-SUM(F2:F232)</f>
-        <v>158731939</v>
-      </c>
-      <c r="G274" s="1">
-        <f>376300000-SUM(G2:G232)</f>
-        <v>177343049</v>
+        <v>475</v>
+      </c>
+      <c r="B274" t="s">
+        <v>476</v>
+      </c>
+      <c r="C274" t="s">
+        <v>441</v>
+      </c>
+      <c r="D274" t="s">
+        <v>442</v>
+      </c>
+      <c r="F274" s="10">
+        <v>365045</v>
+      </c>
+      <c r="G274" s="10">
+        <v>203547</v>
+      </c>
+      <c r="I274" t="s">
+        <v>488</v>
+      </c>
+      <c r="J274" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="275" spans="1:10">
       <c r="A275" t="s">
-        <v>6</v>
-      </c>
-      <c r="F275" s="9">
-        <v>0</v>
-      </c>
-      <c r="G275" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B275" t="s">
+        <v>476</v>
+      </c>
+      <c r="C275" t="s">
+        <v>441</v>
+      </c>
+      <c r="D275" t="s">
+        <v>444</v>
+      </c>
+      <c r="F275" s="10">
+        <v>19915164</v>
+      </c>
+      <c r="G275" s="10">
+        <v>19904018</v>
+      </c>
+      <c r="I275" t="s">
+        <v>488</v>
+      </c>
+      <c r="J275" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="276" spans="1:10">
       <c r="A276" t="s">
-        <v>5</v>
-      </c>
-      <c r="F276" s="9">
-        <v>0</v>
-      </c>
-      <c r="G276" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B276" t="s">
+        <v>476</v>
+      </c>
+      <c r="C276" t="s">
+        <v>441</v>
+      </c>
+      <c r="D276" t="s">
+        <v>443</v>
+      </c>
+      <c r="F276" s="10">
+        <v>2340333</v>
+      </c>
+      <c r="G276" s="10">
+        <v>2362827</v>
+      </c>
+      <c r="I276" t="s">
+        <v>488</v>
+      </c>
+      <c r="J276" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="277" spans="1:10">
       <c r="A277" t="s">
-        <v>4</v>
-      </c>
-      <c r="F277" s="9">
-        <v>0</v>
-      </c>
-      <c r="G277" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B277" t="s">
+        <v>476</v>
+      </c>
+      <c r="C277" t="s">
+        <v>445</v>
+      </c>
+      <c r="D277" t="s">
+        <v>446</v>
+      </c>
+      <c r="F277" s="10">
+        <v>63633</v>
+      </c>
+      <c r="G277" s="10">
+        <v>62438</v>
+      </c>
+      <c r="I277" t="s">
+        <v>488</v>
+      </c>
+      <c r="J277" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="278" spans="1:10">
       <c r="A278" t="s">
-        <v>3</v>
-      </c>
-      <c r="F278" s="9">
-        <v>0</v>
-      </c>
-      <c r="G278" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B278" t="s">
+        <v>476</v>
+      </c>
+      <c r="C278" t="s">
+        <v>445</v>
+      </c>
+      <c r="D278" t="s">
+        <v>447</v>
+      </c>
+      <c r="F278" s="10">
+        <v>167917</v>
+      </c>
+      <c r="G278" s="10">
+        <v>228063</v>
+      </c>
+      <c r="I278" t="s">
+        <v>488</v>
+      </c>
+      <c r="J278" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="279" spans="1:10">
       <c r="A279" t="s">
-        <v>2</v>
-      </c>
-      <c r="F279" s="9">
-        <v>0</v>
-      </c>
-      <c r="G279" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B279" t="s">
+        <v>476</v>
+      </c>
+      <c r="C279" t="s">
+        <v>448</v>
+      </c>
+      <c r="D279" t="s">
+        <v>449</v>
+      </c>
+      <c r="F279" s="10">
+        <v>166925</v>
+      </c>
+      <c r="G279" s="10">
+        <v>178830</v>
+      </c>
+      <c r="H279" t="s">
+        <v>453</v>
+      </c>
+      <c r="I279" t="s">
+        <v>488</v>
+      </c>
+      <c r="J279" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="280" spans="1:10">
       <c r="A280" t="s">
-        <v>203</v>
-      </c>
-      <c r="F280" s="9">
-        <v>0</v>
-      </c>
-      <c r="G280" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B280" t="s">
+        <v>476</v>
+      </c>
+      <c r="C280" t="s">
+        <v>448</v>
+      </c>
+      <c r="D280" t="s">
+        <v>450</v>
+      </c>
+      <c r="F280" s="10">
+        <v>70407</v>
+      </c>
+      <c r="G280" s="10">
+        <v>63543</v>
+      </c>
+      <c r="I280" t="s">
+        <v>488</v>
+      </c>
+      <c r="J280" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="281" spans="1:10">
       <c r="A281" t="s">
-        <v>9</v>
-      </c>
-      <c r="F281" s="9">
-        <v>0</v>
-      </c>
-      <c r="G281" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B281" t="s">
+        <v>476</v>
+      </c>
+      <c r="C281" t="s">
+        <v>448</v>
+      </c>
+      <c r="D281" t="s">
+        <v>451</v>
+      </c>
+      <c r="F281" s="10">
+        <v>82088</v>
+      </c>
+      <c r="G281" s="10">
+        <v>81876</v>
+      </c>
+      <c r="I281" t="s">
+        <v>488</v>
+      </c>
+      <c r="J281" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="282" spans="1:10">
       <c r="A282" t="s">
-        <v>10</v>
-      </c>
-      <c r="F282" s="9">
-        <v>0</v>
-      </c>
-      <c r="G282" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B282" t="s">
+        <v>476</v>
+      </c>
+      <c r="C282" t="s">
+        <v>448</v>
+      </c>
+      <c r="D282" t="s">
+        <v>452</v>
+      </c>
+      <c r="F282" s="10">
+        <v>6139</v>
+      </c>
+      <c r="G282" s="10">
+        <v>6642</v>
+      </c>
+      <c r="I282" t="s">
+        <v>488</v>
+      </c>
+      <c r="J282" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="283" spans="1:10">
       <c r="A283" t="s">
-        <v>11</v>
-      </c>
-      <c r="F283" s="9">
-        <v>0</v>
-      </c>
-      <c r="G283" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B283" t="s">
+        <v>476</v>
+      </c>
+      <c r="C283" t="s">
+        <v>448</v>
+      </c>
+      <c r="D283" t="s">
+        <v>454</v>
+      </c>
+      <c r="F283" s="10">
+        <v>24124</v>
+      </c>
+      <c r="G283" s="10">
+        <v>237138</v>
+      </c>
+      <c r="I283" t="s">
+        <v>488</v>
+      </c>
+      <c r="J283" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="284" spans="1:10">
       <c r="A284" t="s">
-        <v>12</v>
-      </c>
-      <c r="F284" s="9">
-        <v>0</v>
-      </c>
-      <c r="G284" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B284" t="s">
+        <v>476</v>
+      </c>
+      <c r="C284" t="s">
+        <v>455</v>
+      </c>
+      <c r="D284" t="s">
+        <v>456</v>
+      </c>
+      <c r="F284" s="10">
+        <v>34840634</v>
+      </c>
+      <c r="G284" s="10">
+        <v>36800446</v>
+      </c>
+      <c r="I284" t="s">
+        <v>488</v>
+      </c>
+      <c r="J284" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="285" spans="1:10">
       <c r="A285" t="s">
-        <v>13</v>
-      </c>
-      <c r="F285" s="9">
-        <v>0</v>
-      </c>
-      <c r="G285" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B285" t="s">
+        <v>476</v>
+      </c>
+      <c r="C285" t="s">
+        <v>455</v>
+      </c>
+      <c r="D285" t="s">
+        <v>457</v>
+      </c>
+      <c r="F285" s="10">
+        <v>264344</v>
+      </c>
+      <c r="G285" s="10">
+        <v>242267</v>
+      </c>
+      <c r="I285" t="s">
+        <v>488</v>
+      </c>
+      <c r="J285" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="286" spans="1:10">
       <c r="A286" t="s">
-        <v>204</v>
-      </c>
-      <c r="F286" s="9">
-        <v>0</v>
-      </c>
-      <c r="G286" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B286" t="s">
+        <v>476</v>
+      </c>
+      <c r="C286" t="s">
+        <v>458</v>
+      </c>
+      <c r="D286" t="s">
+        <v>459</v>
+      </c>
+      <c r="F286" s="10">
+        <v>166286</v>
+      </c>
+      <c r="G286" s="10">
+        <v>202977</v>
+      </c>
+      <c r="I286" t="s">
+        <v>488</v>
+      </c>
+      <c r="J286" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="287" spans="1:10">
       <c r="A287" t="s">
-        <v>15</v>
-      </c>
-      <c r="F287" s="9">
-        <v>0</v>
-      </c>
-      <c r="G287" s="9">
-        <v>0</v>
+        <v>475</v>
+      </c>
+      <c r="B287" t="s">
+        <v>476</v>
+      </c>
+      <c r="C287" t="s">
+        <v>458</v>
+      </c>
+      <c r="D287" t="s">
+        <v>460</v>
+      </c>
+      <c r="F287" s="10">
+        <v>14519777</v>
+      </c>
+      <c r="G287" s="10">
+        <v>14861857</v>
+      </c>
+      <c r="I287" t="s">
+        <v>488</v>
+      </c>
+      <c r="J287" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
+        <v>475</v>
+      </c>
+      <c r="B288" t="s">
+        <v>476</v>
+      </c>
+      <c r="C288" t="s">
+        <v>458</v>
+      </c>
+      <c r="D288" t="s">
+        <v>461</v>
+      </c>
+      <c r="F288" s="10">
+        <v>5736372</v>
+      </c>
+      <c r="G288" s="10">
+        <v>6291529</v>
+      </c>
+      <c r="I288" t="s">
+        <v>488</v>
+      </c>
+      <c r="J288" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10">
+      <c r="A289" t="s">
+        <v>475</v>
+      </c>
+      <c r="B289" t="s">
+        <v>476</v>
+      </c>
+      <c r="C289" t="s">
+        <v>458</v>
+      </c>
+      <c r="D289" t="s">
+        <v>465</v>
+      </c>
+      <c r="F289" s="10">
+        <v>430529</v>
+      </c>
+      <c r="G289" s="10">
+        <v>360531</v>
+      </c>
+      <c r="I289" t="s">
+        <v>488</v>
+      </c>
+      <c r="J289" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10">
+      <c r="A290" t="s">
+        <v>475</v>
+      </c>
+      <c r="B290" t="s">
+        <v>476</v>
+      </c>
+      <c r="C290" t="s">
+        <v>458</v>
+      </c>
+      <c r="D290" t="s">
+        <v>462</v>
+      </c>
+      <c r="F290" s="10">
+        <v>22359</v>
+      </c>
+      <c r="G290" s="10">
+        <v>21495</v>
+      </c>
+      <c r="I290" t="s">
+        <v>488</v>
+      </c>
+      <c r="J290" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10">
+      <c r="A291" t="s">
+        <v>475</v>
+      </c>
+      <c r="B291" t="s">
+        <v>476</v>
+      </c>
+      <c r="C291" t="s">
+        <v>458</v>
+      </c>
+      <c r="D291" t="s">
+        <v>463</v>
+      </c>
+      <c r="F291" s="10">
+        <v>0</v>
+      </c>
+      <c r="G291" s="10">
+        <v>66921</v>
+      </c>
+      <c r="I291" t="s">
+        <v>488</v>
+      </c>
+      <c r="J291" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="292" spans="1:10">
+      <c r="A292" t="s">
+        <v>475</v>
+      </c>
+      <c r="B292" t="s">
+        <v>476</v>
+      </c>
+      <c r="C292" t="s">
+        <v>458</v>
+      </c>
+      <c r="D292" t="s">
+        <v>464</v>
+      </c>
+      <c r="F292" s="10">
+        <v>0</v>
+      </c>
+      <c r="G292" s="10">
+        <v>96411</v>
+      </c>
+      <c r="I292" t="s">
+        <v>488</v>
+      </c>
+      <c r="J292" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="293" spans="1:10">
+      <c r="A293" t="s">
+        <v>475</v>
+      </c>
+      <c r="B293" t="s">
+        <v>476</v>
+      </c>
+      <c r="C293" t="s">
+        <v>466</v>
+      </c>
+      <c r="F293" s="10">
+        <v>51367</v>
+      </c>
+      <c r="G293" s="10">
+        <v>44242</v>
+      </c>
+      <c r="H293" t="s">
+        <v>467</v>
+      </c>
+      <c r="I293" t="s">
+        <v>488</v>
+      </c>
+      <c r="J293" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="294" spans="1:10">
+      <c r="A294" t="s">
+        <v>475</v>
+      </c>
+      <c r="B294" t="s">
+        <v>476</v>
+      </c>
+      <c r="C294" t="s">
+        <v>468</v>
+      </c>
+      <c r="D294" t="s">
+        <v>469</v>
+      </c>
+      <c r="F294" s="10">
+        <v>300455</v>
+      </c>
+      <c r="G294" s="10">
+        <v>213829</v>
+      </c>
+      <c r="I294" t="s">
+        <v>488</v>
+      </c>
+      <c r="J294" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="295" spans="1:10">
+      <c r="A295" t="s">
+        <v>475</v>
+      </c>
+      <c r="B295" t="s">
+        <v>476</v>
+      </c>
+      <c r="C295" t="s">
+        <v>468</v>
+      </c>
+      <c r="D295" t="s">
+        <v>470</v>
+      </c>
+      <c r="F295" s="10">
+        <v>145312</v>
+      </c>
+      <c r="G295" s="10">
+        <v>102105</v>
+      </c>
+      <c r="I295" t="s">
+        <v>488</v>
+      </c>
+      <c r="J295" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="296" spans="1:10">
+      <c r="A296" t="s">
+        <v>475</v>
+      </c>
+      <c r="B296" t="s">
+        <v>476</v>
+      </c>
+      <c r="C296" t="s">
+        <v>468</v>
+      </c>
+      <c r="D296" t="s">
+        <v>473</v>
+      </c>
+      <c r="F296" s="10">
+        <v>92030</v>
+      </c>
+      <c r="G296" s="10">
+        <v>94567</v>
+      </c>
+      <c r="I296" t="s">
+        <v>488</v>
+      </c>
+      <c r="J296" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10">
+      <c r="A297" t="s">
+        <v>475</v>
+      </c>
+      <c r="B297" t="s">
+        <v>476</v>
+      </c>
+      <c r="C297" t="s">
+        <v>468</v>
+      </c>
+      <c r="D297" t="s">
+        <v>471</v>
+      </c>
+      <c r="F297" s="10">
+        <v>573163</v>
+      </c>
+      <c r="G297" s="10">
+        <v>576908</v>
+      </c>
+      <c r="I297" t="s">
+        <v>488</v>
+      </c>
+      <c r="J297" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="298" spans="1:10">
+      <c r="A298" t="s">
+        <v>475</v>
+      </c>
+      <c r="B298" t="s">
+        <v>476</v>
+      </c>
+      <c r="C298" t="s">
+        <v>468</v>
+      </c>
+      <c r="D298" t="s">
+        <v>472</v>
+      </c>
+      <c r="F298" s="10">
+        <v>140865</v>
+      </c>
+      <c r="G298" s="10">
+        <v>95813</v>
+      </c>
+      <c r="I298" t="s">
+        <v>488</v>
+      </c>
+      <c r="J298" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10">
+      <c r="A299" t="s">
+        <v>475</v>
+      </c>
+      <c r="B299" t="s">
+        <v>474</v>
+      </c>
+      <c r="C299" t="s">
+        <v>478</v>
+      </c>
+      <c r="F299" s="10">
+        <v>53428</v>
+      </c>
+      <c r="G299" s="10">
+        <v>50952</v>
+      </c>
+      <c r="I299" t="s">
+        <v>488</v>
+      </c>
+      <c r="J299" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="300" spans="1:10">
+      <c r="A300" t="s">
+        <v>475</v>
+      </c>
+      <c r="B300" t="s">
+        <v>474</v>
+      </c>
+      <c r="C300" t="s">
+        <v>477</v>
+      </c>
+      <c r="F300" s="10">
+        <v>6500</v>
+      </c>
+      <c r="G300" s="10">
+        <v>4903</v>
+      </c>
+      <c r="I300" t="s">
+        <v>488</v>
+      </c>
+      <c r="J300" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10">
+      <c r="A301" t="s">
+        <v>475</v>
+      </c>
+      <c r="B301" t="s">
+        <v>479</v>
+      </c>
+      <c r="F301" s="10">
+        <v>9956</v>
+      </c>
+      <c r="G301" s="10">
+        <v>10796</v>
+      </c>
+      <c r="I301" t="s">
+        <v>488</v>
+      </c>
+      <c r="J301" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10">
+      <c r="A302" t="s">
+        <v>475</v>
+      </c>
+      <c r="B302" t="s">
+        <v>480</v>
+      </c>
+      <c r="F302" s="10">
+        <v>6110</v>
+      </c>
+      <c r="G302" s="10">
+        <v>5613</v>
+      </c>
+      <c r="I302" t="s">
+        <v>488</v>
+      </c>
+      <c r="J302" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="303" spans="1:10">
+      <c r="A303" t="s">
+        <v>475</v>
+      </c>
+      <c r="B303" t="s">
+        <v>481</v>
+      </c>
+      <c r="C303" t="s">
+        <v>482</v>
+      </c>
+      <c r="F303" s="10">
+        <v>74248</v>
+      </c>
+      <c r="G303" s="10">
+        <v>79835</v>
+      </c>
+      <c r="I303" t="s">
+        <v>488</v>
+      </c>
+      <c r="J303" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10">
+      <c r="A304" t="s">
+        <v>475</v>
+      </c>
+      <c r="B304" t="s">
+        <v>481</v>
+      </c>
+      <c r="C304" t="s">
+        <v>484</v>
+      </c>
+      <c r="F304" s="10">
+        <v>33871</v>
+      </c>
+      <c r="G304" s="10">
+        <v>73869</v>
+      </c>
+      <c r="I304" t="s">
+        <v>488</v>
+      </c>
+      <c r="J304" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="305" spans="1:10">
+      <c r="A305" t="s">
+        <v>475</v>
+      </c>
+      <c r="B305" t="s">
+        <v>481</v>
+      </c>
+      <c r="C305" t="s">
+        <v>483</v>
+      </c>
+      <c r="F305" s="10">
+        <v>34061</v>
+      </c>
+      <c r="G305" s="10">
+        <v>32274</v>
+      </c>
+      <c r="I305" t="s">
+        <v>488</v>
+      </c>
+      <c r="J305" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="306" spans="1:10">
+      <c r="A306" t="s">
+        <v>475</v>
+      </c>
+      <c r="B306" t="s">
+        <v>485</v>
+      </c>
+      <c r="F306" s="10">
+        <v>84175</v>
+      </c>
+      <c r="G306" s="10">
+        <v>74015</v>
+      </c>
+      <c r="I306" t="s">
+        <v>488</v>
+      </c>
+      <c r="J306" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10">
+      <c r="A307" t="s">
+        <v>475</v>
+      </c>
+      <c r="B307" t="s">
+        <v>486</v>
+      </c>
+      <c r="F307" s="10">
+        <v>57517</v>
+      </c>
+      <c r="G307" s="10">
+        <v>72219</v>
+      </c>
+      <c r="I307" t="s">
+        <v>488</v>
+      </c>
+      <c r="J307" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="308" spans="1:10">
+      <c r="A308" t="s">
+        <v>490</v>
+      </c>
+      <c r="B308" t="s">
+        <v>491</v>
+      </c>
+      <c r="C308" t="s">
+        <v>492</v>
+      </c>
+      <c r="D308" t="s">
+        <v>493</v>
+      </c>
+      <c r="E308" t="s">
+        <v>496</v>
+      </c>
+      <c r="F308" s="10">
+        <v>395573</v>
+      </c>
+      <c r="G308" s="10">
+        <v>379205</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10">
+      <c r="B309" t="s">
+        <v>491</v>
+      </c>
+      <c r="C309" t="s">
+        <v>492</v>
+      </c>
+      <c r="D309" t="s">
+        <v>493</v>
+      </c>
+      <c r="E309" t="s">
+        <v>497</v>
+      </c>
+      <c r="F309" s="10">
+        <v>5980</v>
+      </c>
+      <c r="G309" s="10">
+        <v>77400</v>
+      </c>
+    </row>
+    <row r="310" spans="1:10">
+      <c r="B310" t="s">
+        <v>491</v>
+      </c>
+      <c r="C310" t="s">
+        <v>492</v>
+      </c>
+      <c r="D310" t="s">
+        <v>493</v>
+      </c>
+      <c r="E310" t="s">
+        <v>498</v>
+      </c>
+      <c r="F310" s="10">
+        <v>28175</v>
+      </c>
+      <c r="G310" s="10">
+        <v>26100</v>
+      </c>
+    </row>
+    <row r="311" spans="1:10">
+      <c r="B311" t="s">
+        <v>491</v>
+      </c>
+      <c r="C311" t="s">
+        <v>492</v>
+      </c>
+      <c r="D311" t="s">
+        <v>493</v>
+      </c>
+      <c r="E311" t="s">
+        <v>387</v>
+      </c>
+      <c r="F311" s="10">
+        <f>816169-SUM(F308:F310)</f>
+        <v>386441</v>
+      </c>
+      <c r="G311" s="10">
+        <f>685151-SUM(G308:G310)</f>
+        <v>202446</v>
+      </c>
+    </row>
+    <row r="312" spans="1:10">
+      <c r="A312" t="s">
+        <v>490</v>
+      </c>
+      <c r="B312" t="s">
+        <v>491</v>
+      </c>
+      <c r="C312" t="s">
+        <v>492</v>
+      </c>
+      <c r="D312" t="s">
+        <v>495</v>
+      </c>
+      <c r="E312" t="s">
+        <v>499</v>
+      </c>
+      <c r="F312" s="10">
+        <v>165724</v>
+      </c>
+      <c r="G312" s="10">
+        <v>154493</v>
+      </c>
+    </row>
+    <row r="313" spans="1:10">
+      <c r="B313" t="s">
+        <v>491</v>
+      </c>
+      <c r="C313" t="s">
+        <v>492</v>
+      </c>
+      <c r="D313" t="s">
+        <v>495</v>
+      </c>
+      <c r="E313" t="s">
+        <v>500</v>
+      </c>
+      <c r="F313" s="10">
+        <v>125542</v>
+      </c>
+      <c r="G313" s="10">
+        <v>57780</v>
+      </c>
+    </row>
+    <row r="314" spans="1:10">
+      <c r="B314" t="s">
+        <v>491</v>
+      </c>
+      <c r="C314" t="s">
+        <v>492</v>
+      </c>
+      <c r="D314" t="s">
+        <v>495</v>
+      </c>
+      <c r="E314" t="s">
+        <v>501</v>
+      </c>
+      <c r="F314" s="10">
+        <v>57300</v>
+      </c>
+      <c r="G314" s="10">
+        <v>69684</v>
+      </c>
+    </row>
+    <row r="315" spans="1:10">
+      <c r="B315" t="s">
+        <v>491</v>
+      </c>
+      <c r="C315" t="s">
+        <v>492</v>
+      </c>
+      <c r="D315" t="s">
+        <v>495</v>
+      </c>
+      <c r="E315" t="s">
+        <v>387</v>
+      </c>
+      <c r="F315" s="10">
+        <f>378840-SUM(F312:F314)</f>
+        <v>30274</v>
+      </c>
+      <c r="G315" s="10">
+        <f>312731-SUM(G312:G314)</f>
+        <v>30774</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10">
+      <c r="A316" t="s">
+        <v>490</v>
+      </c>
+      <c r="B316" t="s">
+        <v>491</v>
+      </c>
+      <c r="C316" t="s">
+        <v>492</v>
+      </c>
+      <c r="D316" t="s">
+        <v>494</v>
+      </c>
+      <c r="F316" s="10">
+        <v>351620</v>
+      </c>
+      <c r="G316" s="10">
+        <v>340464</v>
+      </c>
+    </row>
+    <row r="317" spans="1:10">
+      <c r="A317" t="s">
+        <v>490</v>
+      </c>
+      <c r="B317" t="s">
+        <v>491</v>
+      </c>
+      <c r="C317" t="s">
+        <v>502</v>
+      </c>
+      <c r="D317" t="s">
+        <v>503</v>
+      </c>
+      <c r="E317" t="s">
+        <v>506</v>
+      </c>
+      <c r="F317" s="10">
+        <v>20727</v>
+      </c>
+      <c r="G317" s="10">
+        <v>21525</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10">
+      <c r="A318" t="s">
+        <v>490</v>
+      </c>
+      <c r="B318" t="s">
+        <v>491</v>
+      </c>
+      <c r="C318" t="s">
+        <v>502</v>
+      </c>
+      <c r="D318" t="s">
+        <v>503</v>
+      </c>
+      <c r="E318" t="s">
+        <v>505</v>
+      </c>
+      <c r="F318" s="10">
+        <v>332489</v>
+      </c>
+      <c r="G318" s="10">
+        <v>345293</v>
+      </c>
+    </row>
+    <row r="319" spans="1:10">
+      <c r="A319" t="s">
+        <v>490</v>
+      </c>
+      <c r="B319" t="s">
+        <v>491</v>
+      </c>
+      <c r="C319" t="s">
+        <v>502</v>
+      </c>
+      <c r="D319" t="s">
+        <v>503</v>
+      </c>
+      <c r="E319" t="s">
+        <v>507</v>
+      </c>
+      <c r="F319" s="10">
+        <v>224467</v>
+      </c>
+      <c r="G319" s="10">
+        <v>233111</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10">
+      <c r="A320" t="s">
+        <v>490</v>
+      </c>
+      <c r="B320" t="s">
+        <v>491</v>
+      </c>
+      <c r="C320" t="s">
+        <v>502</v>
+      </c>
+      <c r="D320" t="s">
+        <v>503</v>
+      </c>
+      <c r="E320" t="s">
+        <v>508</v>
+      </c>
+      <c r="F320" s="10">
+        <v>631763</v>
+      </c>
+      <c r="G320" s="10">
+        <v>656092</v>
+      </c>
+    </row>
+    <row r="321" spans="1:7">
+      <c r="A321" t="s">
+        <v>490</v>
+      </c>
+      <c r="B321" t="s">
+        <v>491</v>
+      </c>
+      <c r="C321" t="s">
+        <v>502</v>
+      </c>
+      <c r="D321" t="s">
+        <v>503</v>
+      </c>
+      <c r="E321" t="s">
+        <v>509</v>
+      </c>
+      <c r="F321" s="10">
+        <v>165193</v>
+      </c>
+      <c r="G321" s="10">
+        <v>218593</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7">
+      <c r="A322" t="s">
+        <v>490</v>
+      </c>
+      <c r="B322" t="s">
+        <v>491</v>
+      </c>
+      <c r="C322" t="s">
+        <v>502</v>
+      </c>
+      <c r="D322" t="s">
+        <v>503</v>
+      </c>
+      <c r="E322" t="s">
+        <v>510</v>
+      </c>
+      <c r="F322" s="10">
+        <v>218867</v>
+      </c>
+      <c r="G322" s="10">
+        <v>248368</v>
+      </c>
+    </row>
+    <row r="323" spans="1:7">
+      <c r="A323" t="s">
+        <v>490</v>
+      </c>
+      <c r="B323" t="s">
+        <v>491</v>
+      </c>
+      <c r="C323" t="s">
+        <v>502</v>
+      </c>
+      <c r="D323" t="s">
+        <v>503</v>
+      </c>
+      <c r="E323" t="s">
+        <v>511</v>
+      </c>
+      <c r="F323" s="10">
+        <v>2863</v>
+      </c>
+      <c r="G323" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:7">
+      <c r="A324" t="s">
+        <v>490</v>
+      </c>
+      <c r="B324" t="s">
+        <v>491</v>
+      </c>
+      <c r="C324" t="s">
+        <v>502</v>
+      </c>
+      <c r="D324" t="s">
+        <v>504</v>
+      </c>
+      <c r="F324" s="10">
+        <v>463698</v>
+      </c>
+      <c r="G324" s="10">
+        <v>362943</v>
+      </c>
+    </row>
+    <row r="325" spans="1:7">
+      <c r="A325" t="s">
+        <v>490</v>
+      </c>
+      <c r="B325" t="s">
+        <v>491</v>
+      </c>
+      <c r="C325" t="s">
+        <v>502</v>
+      </c>
+      <c r="D325" t="s">
+        <v>494</v>
+      </c>
+      <c r="F325" s="10">
+        <v>78662</v>
+      </c>
+      <c r="G325" s="10">
+        <v>72207</v>
+      </c>
+    </row>
+    <row r="326" spans="1:7">
+      <c r="F326" s="10"/>
+      <c r="G326" s="10"/>
+    </row>
+    <row r="327" spans="1:7">
+      <c r="F327" s="10"/>
+      <c r="G327" s="10"/>
+    </row>
+    <row r="328" spans="1:7">
+      <c r="F328" s="10"/>
+      <c r="G328" s="10"/>
+    </row>
+    <row r="329" spans="1:7">
+      <c r="F329" s="10"/>
+      <c r="G329" s="10"/>
+    </row>
+    <row r="330" spans="1:7">
+      <c r="F330" s="10"/>
+      <c r="G330" s="10"/>
+    </row>
+    <row r="331" spans="1:7">
+      <c r="F331" s="14"/>
+      <c r="G331" s="14"/>
+    </row>
+    <row r="332" spans="1:7">
+      <c r="A332" t="s">
+        <v>489</v>
+      </c>
+      <c r="F332" s="1">
+        <f>365800000-SUM(F2:F331)</f>
+        <v>37204026</v>
+      </c>
+      <c r="G332" s="1">
+        <f>376300000-SUM(G2:G331)</f>
+        <v>53706693</v>
+      </c>
+    </row>
+    <row r="333" spans="1:7">
+      <c r="A333" t="s">
+        <v>6</v>
+      </c>
+      <c r="F333" s="9">
+        <v>0</v>
+      </c>
+      <c r="G333" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7">
+      <c r="A334" t="s">
+        <v>5</v>
+      </c>
+      <c r="F334" s="9">
+        <v>0</v>
+      </c>
+      <c r="G334" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="335" spans="1:7">
+      <c r="A335" t="s">
+        <v>4</v>
+      </c>
+      <c r="F335" s="9">
+        <v>0</v>
+      </c>
+      <c r="G335" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="336" spans="1:7">
+      <c r="A336" t="s">
+        <v>3</v>
+      </c>
+      <c r="F336" s="9">
+        <v>0</v>
+      </c>
+      <c r="G336" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="337" spans="1:7">
+      <c r="A337" t="s">
+        <v>2</v>
+      </c>
+      <c r="F337" s="9">
+        <v>0</v>
+      </c>
+      <c r="G337" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="338" spans="1:7">
+      <c r="A338" t="s">
+        <v>9</v>
+      </c>
+      <c r="F338" s="9">
+        <v>0</v>
+      </c>
+      <c r="G338" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="339" spans="1:7">
+      <c r="A339" t="s">
+        <v>10</v>
+      </c>
+      <c r="F339" s="9">
+        <v>0</v>
+      </c>
+      <c r="G339" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7">
+      <c r="A340" t="s">
+        <v>12</v>
+      </c>
+      <c r="F340" s="9">
+        <v>0</v>
+      </c>
+      <c r="G340" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="341" spans="1:7">
+      <c r="A341" t="s">
+        <v>13</v>
+      </c>
+      <c r="F341" s="9">
+        <v>0</v>
+      </c>
+      <c r="G341" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="342" spans="1:7">
+      <c r="A342" t="s">
+        <v>15</v>
+      </c>
+      <c r="F342" s="9">
+        <v>0</v>
+      </c>
+      <c r="G342" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="343" spans="1:7">
+      <c r="A343" t="s">
         <v>16</v>
       </c>
-      <c r="F288" s="9">
-        <v>0</v>
-      </c>
-      <c r="G288" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="289" spans="1:7">
-      <c r="A289" t="s">
+      <c r="F343" s="9">
+        <v>0</v>
+      </c>
+      <c r="G343" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="344" spans="1:7">
+      <c r="A344" t="s">
         <v>205</v>
       </c>
-      <c r="F289" s="9">
-        <v>0</v>
-      </c>
-      <c r="G289" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="290" spans="1:7">
-      <c r="A290" t="s">
+      <c r="F344" s="9">
+        <v>0</v>
+      </c>
+      <c r="G344" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="345" spans="1:7">
+      <c r="A345" t="s">
         <v>18</v>
       </c>
-      <c r="F290" s="9">
-        <v>0</v>
-      </c>
-      <c r="G290" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="291" spans="1:7">
-      <c r="A291" t="s">
+      <c r="F345" s="9">
+        <v>0</v>
+      </c>
+      <c r="G345" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7">
+      <c r="A346" t="s">
         <v>206</v>
       </c>
-      <c r="F291" s="9">
-        <v>0</v>
-      </c>
-      <c r="G291" s="9">
+      <c r="F346" s="9">
+        <v>0</v>
+      </c>
+      <c r="G346" s="9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added narrow version of site
</commit_message>
<xml_diff>
--- a/public/budget_data.xlsx
+++ b/public/budget_data.xlsx
@@ -331,7 +331,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3380" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3386" uniqueCount="512">
   <si>
     <t>-</t>
   </si>
@@ -1766,9 +1766,6 @@
     <t>Aboriginal Hostels Limited</t>
   </si>
   <si>
-    <t>Families, Housing, Community Services and indigenous affairs portfolio</t>
-  </si>
-  <si>
     <t>Department of Families, Housing, Community Services and indigenous affairs</t>
   </si>
   <si>
@@ -1875,6 +1872,9 @@
   </si>
   <si>
     <t>The Commercialisation Training Scheme</t>
+  </si>
+  <si>
+    <t>Families, Housing, Community Services and Indigenous Affairs portfolio</t>
   </si>
 </sst>
 </file>
@@ -1976,8 +1976,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="645">
+  <cellStyleXfs count="649">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2647,7 +2651,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="645">
+  <cellStyles count="649">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2970,6 +2974,8 @@
     <cellStyle name="Followed Hyperlink" xfId="640" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="642" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="644" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="646" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="648" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3292,6 +3298,8 @@
     <cellStyle name="Hyperlink" xfId="639" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="641" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="643" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="645" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="647" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4620,8 +4628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
-      <selection activeCell="B338" sqref="B338"/>
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
+      <selection activeCell="A274" sqref="A274:A307"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11446,10 +11454,10 @@
     </row>
     <row r="274" spans="1:10">
       <c r="A274" t="s">
+        <v>511</v>
+      </c>
+      <c r="B274" t="s">
         <v>475</v>
-      </c>
-      <c r="B274" t="s">
-        <v>476</v>
       </c>
       <c r="C274" t="s">
         <v>441</v>
@@ -11464,18 +11472,18 @@
         <v>203547</v>
       </c>
       <c r="I274" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J274" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="275" spans="1:10">
       <c r="A275" t="s">
+        <v>511</v>
+      </c>
+      <c r="B275" t="s">
         <v>475</v>
-      </c>
-      <c r="B275" t="s">
-        <v>476</v>
       </c>
       <c r="C275" t="s">
         <v>441</v>
@@ -11490,18 +11498,18 @@
         <v>19904018</v>
       </c>
       <c r="I275" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J275" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="276" spans="1:10">
       <c r="A276" t="s">
+        <v>511</v>
+      </c>
+      <c r="B276" t="s">
         <v>475</v>
-      </c>
-      <c r="B276" t="s">
-        <v>476</v>
       </c>
       <c r="C276" t="s">
         <v>441</v>
@@ -11516,18 +11524,18 @@
         <v>2362827</v>
       </c>
       <c r="I276" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J276" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="277" spans="1:10">
       <c r="A277" t="s">
+        <v>511</v>
+      </c>
+      <c r="B277" t="s">
         <v>475</v>
-      </c>
-      <c r="B277" t="s">
-        <v>476</v>
       </c>
       <c r="C277" t="s">
         <v>445</v>
@@ -11542,18 +11550,18 @@
         <v>62438</v>
       </c>
       <c r="I277" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J277" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="278" spans="1:10">
       <c r="A278" t="s">
+        <v>511</v>
+      </c>
+      <c r="B278" t="s">
         <v>475</v>
-      </c>
-      <c r="B278" t="s">
-        <v>476</v>
       </c>
       <c r="C278" t="s">
         <v>445</v>
@@ -11568,18 +11576,18 @@
         <v>228063</v>
       </c>
       <c r="I278" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J278" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="279" spans="1:10">
       <c r="A279" t="s">
+        <v>511</v>
+      </c>
+      <c r="B279" t="s">
         <v>475</v>
-      </c>
-      <c r="B279" t="s">
-        <v>476</v>
       </c>
       <c r="C279" t="s">
         <v>448</v>
@@ -11597,18 +11605,18 @@
         <v>453</v>
       </c>
       <c r="I279" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J279" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="280" spans="1:10">
       <c r="A280" t="s">
+        <v>511</v>
+      </c>
+      <c r="B280" t="s">
         <v>475</v>
-      </c>
-      <c r="B280" t="s">
-        <v>476</v>
       </c>
       <c r="C280" t="s">
         <v>448</v>
@@ -11623,18 +11631,18 @@
         <v>63543</v>
       </c>
       <c r="I280" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J280" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="281" spans="1:10">
       <c r="A281" t="s">
+        <v>511</v>
+      </c>
+      <c r="B281" t="s">
         <v>475</v>
-      </c>
-      <c r="B281" t="s">
-        <v>476</v>
       </c>
       <c r="C281" t="s">
         <v>448</v>
@@ -11649,18 +11657,18 @@
         <v>81876</v>
       </c>
       <c r="I281" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J281" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="282" spans="1:10">
       <c r="A282" t="s">
+        <v>511</v>
+      </c>
+      <c r="B282" t="s">
         <v>475</v>
-      </c>
-      <c r="B282" t="s">
-        <v>476</v>
       </c>
       <c r="C282" t="s">
         <v>448</v>
@@ -11675,18 +11683,18 @@
         <v>6642</v>
       </c>
       <c r="I282" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J282" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="283" spans="1:10">
       <c r="A283" t="s">
+        <v>511</v>
+      </c>
+      <c r="B283" t="s">
         <v>475</v>
-      </c>
-      <c r="B283" t="s">
-        <v>476</v>
       </c>
       <c r="C283" t="s">
         <v>448</v>
@@ -11701,18 +11709,18 @@
         <v>237138</v>
       </c>
       <c r="I283" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J283" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="284" spans="1:10">
       <c r="A284" t="s">
+        <v>511</v>
+      </c>
+      <c r="B284" t="s">
         <v>475</v>
-      </c>
-      <c r="B284" t="s">
-        <v>476</v>
       </c>
       <c r="C284" t="s">
         <v>455</v>
@@ -11727,18 +11735,18 @@
         <v>36800446</v>
       </c>
       <c r="I284" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J284" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="285" spans="1:10">
       <c r="A285" t="s">
+        <v>511</v>
+      </c>
+      <c r="B285" t="s">
         <v>475</v>
-      </c>
-      <c r="B285" t="s">
-        <v>476</v>
       </c>
       <c r="C285" t="s">
         <v>455</v>
@@ -11753,18 +11761,18 @@
         <v>242267</v>
       </c>
       <c r="I285" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J285" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="286" spans="1:10">
       <c r="A286" t="s">
+        <v>511</v>
+      </c>
+      <c r="B286" t="s">
         <v>475</v>
-      </c>
-      <c r="B286" t="s">
-        <v>476</v>
       </c>
       <c r="C286" t="s">
         <v>458</v>
@@ -11779,18 +11787,18 @@
         <v>202977</v>
       </c>
       <c r="I286" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J286" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="287" spans="1:10">
       <c r="A287" t="s">
+        <v>511</v>
+      </c>
+      <c r="B287" t="s">
         <v>475</v>
-      </c>
-      <c r="B287" t="s">
-        <v>476</v>
       </c>
       <c r="C287" t="s">
         <v>458</v>
@@ -11805,18 +11813,18 @@
         <v>14861857</v>
       </c>
       <c r="I287" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J287" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="288" spans="1:10">
       <c r="A288" t="s">
+        <v>511</v>
+      </c>
+      <c r="B288" t="s">
         <v>475</v>
-      </c>
-      <c r="B288" t="s">
-        <v>476</v>
       </c>
       <c r="C288" t="s">
         <v>458</v>
@@ -11831,18 +11839,18 @@
         <v>6291529</v>
       </c>
       <c r="I288" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J288" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="289" spans="1:10">
       <c r="A289" t="s">
+        <v>511</v>
+      </c>
+      <c r="B289" t="s">
         <v>475</v>
-      </c>
-      <c r="B289" t="s">
-        <v>476</v>
       </c>
       <c r="C289" t="s">
         <v>458</v>
@@ -11857,18 +11865,18 @@
         <v>360531</v>
       </c>
       <c r="I289" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J289" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="290" spans="1:10">
       <c r="A290" t="s">
+        <v>511</v>
+      </c>
+      <c r="B290" t="s">
         <v>475</v>
-      </c>
-      <c r="B290" t="s">
-        <v>476</v>
       </c>
       <c r="C290" t="s">
         <v>458</v>
@@ -11883,18 +11891,18 @@
         <v>21495</v>
       </c>
       <c r="I290" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J290" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="291" spans="1:10">
       <c r="A291" t="s">
+        <v>511</v>
+      </c>
+      <c r="B291" t="s">
         <v>475</v>
-      </c>
-      <c r="B291" t="s">
-        <v>476</v>
       </c>
       <c r="C291" t="s">
         <v>458</v>
@@ -11909,18 +11917,18 @@
         <v>66921</v>
       </c>
       <c r="I291" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J291" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="292" spans="1:10">
       <c r="A292" t="s">
+        <v>511</v>
+      </c>
+      <c r="B292" t="s">
         <v>475</v>
-      </c>
-      <c r="B292" t="s">
-        <v>476</v>
       </c>
       <c r="C292" t="s">
         <v>458</v>
@@ -11935,18 +11943,18 @@
         <v>96411</v>
       </c>
       <c r="I292" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J292" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="293" spans="1:10">
       <c r="A293" t="s">
+        <v>511</v>
+      </c>
+      <c r="B293" t="s">
         <v>475</v>
-      </c>
-      <c r="B293" t="s">
-        <v>476</v>
       </c>
       <c r="C293" t="s">
         <v>466</v>
@@ -11961,18 +11969,18 @@
         <v>467</v>
       </c>
       <c r="I293" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J293" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="294" spans="1:10">
       <c r="A294" t="s">
+        <v>511</v>
+      </c>
+      <c r="B294" t="s">
         <v>475</v>
-      </c>
-      <c r="B294" t="s">
-        <v>476</v>
       </c>
       <c r="C294" t="s">
         <v>468</v>
@@ -11987,18 +11995,18 @@
         <v>213829</v>
       </c>
       <c r="I294" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J294" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="295" spans="1:10">
       <c r="A295" t="s">
+        <v>511</v>
+      </c>
+      <c r="B295" t="s">
         <v>475</v>
-      </c>
-      <c r="B295" t="s">
-        <v>476</v>
       </c>
       <c r="C295" t="s">
         <v>468</v>
@@ -12013,18 +12021,18 @@
         <v>102105</v>
       </c>
       <c r="I295" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J295" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="296" spans="1:10">
       <c r="A296" t="s">
+        <v>511</v>
+      </c>
+      <c r="B296" t="s">
         <v>475</v>
-      </c>
-      <c r="B296" t="s">
-        <v>476</v>
       </c>
       <c r="C296" t="s">
         <v>468</v>
@@ -12039,18 +12047,18 @@
         <v>94567</v>
       </c>
       <c r="I296" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J296" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="297" spans="1:10">
       <c r="A297" t="s">
+        <v>511</v>
+      </c>
+      <c r="B297" t="s">
         <v>475</v>
-      </c>
-      <c r="B297" t="s">
-        <v>476</v>
       </c>
       <c r="C297" t="s">
         <v>468</v>
@@ -12065,18 +12073,18 @@
         <v>576908</v>
       </c>
       <c r="I297" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J297" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="298" spans="1:10">
       <c r="A298" t="s">
+        <v>511</v>
+      </c>
+      <c r="B298" t="s">
         <v>475</v>
-      </c>
-      <c r="B298" t="s">
-        <v>476</v>
       </c>
       <c r="C298" t="s">
         <v>468</v>
@@ -12091,21 +12099,21 @@
         <v>95813</v>
       </c>
       <c r="I298" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J298" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="299" spans="1:10">
       <c r="A299" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B299" t="s">
         <v>474</v>
       </c>
       <c r="C299" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F299" s="10">
         <v>53428</v>
@@ -12114,21 +12122,21 @@
         <v>50952</v>
       </c>
       <c r="I299" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J299" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="300" spans="1:10">
       <c r="A300" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B300" t="s">
         <v>474</v>
       </c>
       <c r="C300" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F300" s="10">
         <v>6500</v>
@@ -12137,18 +12145,18 @@
         <v>4903</v>
       </c>
       <c r="I300" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J300" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="301" spans="1:10">
       <c r="A301" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B301" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F301" s="10">
         <v>9956</v>
@@ -12157,18 +12165,18 @@
         <v>10796</v>
       </c>
       <c r="I301" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J301" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="302" spans="1:10">
       <c r="A302" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B302" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F302" s="10">
         <v>6110</v>
@@ -12177,21 +12185,21 @@
         <v>5613</v>
       </c>
       <c r="I302" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J302" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="303" spans="1:10">
       <c r="A303" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B303" t="s">
+        <v>480</v>
+      </c>
+      <c r="C303" t="s">
         <v>481</v>
-      </c>
-      <c r="C303" t="s">
-        <v>482</v>
       </c>
       <c r="F303" s="10">
         <v>74248</v>
@@ -12200,21 +12208,21 @@
         <v>79835</v>
       </c>
       <c r="I303" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J303" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="304" spans="1:10">
       <c r="A304" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B304" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C304" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F304" s="10">
         <v>33871</v>
@@ -12223,21 +12231,21 @@
         <v>73869</v>
       </c>
       <c r="I304" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J304" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="305" spans="1:10">
       <c r="A305" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B305" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C305" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F305" s="10">
         <v>34061</v>
@@ -12246,18 +12254,18 @@
         <v>32274</v>
       </c>
       <c r="I305" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J305" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="306" spans="1:10">
       <c r="A306" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B306" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F306" s="10">
         <v>84175</v>
@@ -12266,18 +12274,18 @@
         <v>74015</v>
       </c>
       <c r="I306" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J306" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="307" spans="1:10">
       <c r="A307" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="B307" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="F307" s="10">
         <v>57517</v>
@@ -12286,27 +12294,27 @@
         <v>72219</v>
       </c>
       <c r="I307" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="J307" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="308" spans="1:10">
       <c r="A308" t="s">
+        <v>489</v>
+      </c>
+      <c r="B308" t="s">
         <v>490</v>
       </c>
-      <c r="B308" t="s">
+      <c r="C308" t="s">
         <v>491</v>
       </c>
-      <c r="C308" t="s">
+      <c r="D308" t="s">
         <v>492</v>
       </c>
-      <c r="D308" t="s">
-        <v>493</v>
-      </c>
       <c r="E308" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F308" s="10">
         <v>395573</v>
@@ -12316,17 +12324,20 @@
       </c>
     </row>
     <row r="309" spans="1:10">
+      <c r="A309" t="s">
+        <v>489</v>
+      </c>
       <c r="B309" t="s">
+        <v>490</v>
+      </c>
+      <c r="C309" t="s">
         <v>491</v>
       </c>
-      <c r="C309" t="s">
+      <c r="D309" t="s">
         <v>492</v>
       </c>
-      <c r="D309" t="s">
-        <v>493</v>
-      </c>
       <c r="E309" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F309" s="10">
         <v>5980</v>
@@ -12336,17 +12347,20 @@
       </c>
     </row>
     <row r="310" spans="1:10">
+      <c r="A310" t="s">
+        <v>489</v>
+      </c>
       <c r="B310" t="s">
+        <v>490</v>
+      </c>
+      <c r="C310" t="s">
         <v>491</v>
       </c>
-      <c r="C310" t="s">
+      <c r="D310" t="s">
         <v>492</v>
       </c>
-      <c r="D310" t="s">
-        <v>493</v>
-      </c>
       <c r="E310" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F310" s="10">
         <v>28175</v>
@@ -12356,14 +12370,17 @@
       </c>
     </row>
     <row r="311" spans="1:10">
+      <c r="A311" t="s">
+        <v>489</v>
+      </c>
       <c r="B311" t="s">
+        <v>490</v>
+      </c>
+      <c r="C311" t="s">
         <v>491</v>
       </c>
-      <c r="C311" t="s">
+      <c r="D311" t="s">
         <v>492</v>
-      </c>
-      <c r="D311" t="s">
-        <v>493</v>
       </c>
       <c r="E311" t="s">
         <v>387</v>
@@ -12379,19 +12396,19 @@
     </row>
     <row r="312" spans="1:10">
       <c r="A312" t="s">
+        <v>489</v>
+      </c>
+      <c r="B312" t="s">
         <v>490</v>
       </c>
-      <c r="B312" t="s">
+      <c r="C312" t="s">
         <v>491</v>
       </c>
-      <c r="C312" t="s">
-        <v>492</v>
-      </c>
       <c r="D312" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E312" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F312" s="10">
         <v>165724</v>
@@ -12401,17 +12418,20 @@
       </c>
     </row>
     <row r="313" spans="1:10">
+      <c r="A313" t="s">
+        <v>489</v>
+      </c>
       <c r="B313" t="s">
+        <v>490</v>
+      </c>
+      <c r="C313" t="s">
         <v>491</v>
       </c>
-      <c r="C313" t="s">
-        <v>492</v>
-      </c>
       <c r="D313" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E313" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F313" s="10">
         <v>125542</v>
@@ -12421,17 +12441,20 @@
       </c>
     </row>
     <row r="314" spans="1:10">
+      <c r="A314" t="s">
+        <v>489</v>
+      </c>
       <c r="B314" t="s">
+        <v>490</v>
+      </c>
+      <c r="C314" t="s">
         <v>491</v>
       </c>
-      <c r="C314" t="s">
-        <v>492</v>
-      </c>
       <c r="D314" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E314" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F314" s="10">
         <v>57300</v>
@@ -12441,14 +12464,17 @@
       </c>
     </row>
     <row r="315" spans="1:10">
+      <c r="A315" t="s">
+        <v>489</v>
+      </c>
       <c r="B315" t="s">
+        <v>490</v>
+      </c>
+      <c r="C315" t="s">
         <v>491</v>
       </c>
-      <c r="C315" t="s">
-        <v>492</v>
-      </c>
       <c r="D315" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E315" t="s">
         <v>387</v>
@@ -12464,16 +12490,16 @@
     </row>
     <row r="316" spans="1:10">
       <c r="A316" t="s">
+        <v>489</v>
+      </c>
+      <c r="B316" t="s">
         <v>490</v>
       </c>
-      <c r="B316" t="s">
+      <c r="C316" t="s">
         <v>491</v>
       </c>
-      <c r="C316" t="s">
-        <v>492</v>
-      </c>
       <c r="D316" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F316" s="10">
         <v>351620</v>
@@ -12484,19 +12510,19 @@
     </row>
     <row r="317" spans="1:10">
       <c r="A317" t="s">
+        <v>489</v>
+      </c>
+      <c r="B317" t="s">
         <v>490</v>
       </c>
-      <c r="B317" t="s">
-        <v>491</v>
-      </c>
       <c r="C317" t="s">
+        <v>501</v>
+      </c>
+      <c r="D317" t="s">
         <v>502</v>
       </c>
-      <c r="D317" t="s">
-        <v>503</v>
-      </c>
       <c r="E317" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F317" s="10">
         <v>20727</v>
@@ -12507,19 +12533,19 @@
     </row>
     <row r="318" spans="1:10">
       <c r="A318" t="s">
+        <v>489</v>
+      </c>
+      <c r="B318" t="s">
         <v>490</v>
       </c>
-      <c r="B318" t="s">
-        <v>491</v>
-      </c>
       <c r="C318" t="s">
+        <v>501</v>
+      </c>
+      <c r="D318" t="s">
         <v>502</v>
       </c>
-      <c r="D318" t="s">
-        <v>503</v>
-      </c>
       <c r="E318" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F318" s="10">
         <v>332489</v>
@@ -12530,19 +12556,19 @@
     </row>
     <row r="319" spans="1:10">
       <c r="A319" t="s">
+        <v>489</v>
+      </c>
+      <c r="B319" t="s">
         <v>490</v>
       </c>
-      <c r="B319" t="s">
-        <v>491</v>
-      </c>
       <c r="C319" t="s">
+        <v>501</v>
+      </c>
+      <c r="D319" t="s">
         <v>502</v>
       </c>
-      <c r="D319" t="s">
-        <v>503</v>
-      </c>
       <c r="E319" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F319" s="10">
         <v>224467</v>
@@ -12553,19 +12579,19 @@
     </row>
     <row r="320" spans="1:10">
       <c r="A320" t="s">
+        <v>489</v>
+      </c>
+      <c r="B320" t="s">
         <v>490</v>
       </c>
-      <c r="B320" t="s">
-        <v>491</v>
-      </c>
       <c r="C320" t="s">
+        <v>501</v>
+      </c>
+      <c r="D320" t="s">
         <v>502</v>
       </c>
-      <c r="D320" t="s">
-        <v>503</v>
-      </c>
       <c r="E320" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F320" s="10">
         <v>631763</v>
@@ -12576,19 +12602,19 @@
     </row>
     <row r="321" spans="1:7">
       <c r="A321" t="s">
+        <v>489</v>
+      </c>
+      <c r="B321" t="s">
         <v>490</v>
       </c>
-      <c r="B321" t="s">
-        <v>491</v>
-      </c>
       <c r="C321" t="s">
+        <v>501</v>
+      </c>
+      <c r="D321" t="s">
         <v>502</v>
       </c>
-      <c r="D321" t="s">
-        <v>503</v>
-      </c>
       <c r="E321" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F321" s="10">
         <v>165193</v>
@@ -12599,19 +12625,19 @@
     </row>
     <row r="322" spans="1:7">
       <c r="A322" t="s">
+        <v>489</v>
+      </c>
+      <c r="B322" t="s">
         <v>490</v>
       </c>
-      <c r="B322" t="s">
-        <v>491</v>
-      </c>
       <c r="C322" t="s">
+        <v>501</v>
+      </c>
+      <c r="D322" t="s">
         <v>502</v>
       </c>
-      <c r="D322" t="s">
-        <v>503</v>
-      </c>
       <c r="E322" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F322" s="10">
         <v>218867</v>
@@ -12622,19 +12648,19 @@
     </row>
     <row r="323" spans="1:7">
       <c r="A323" t="s">
+        <v>489</v>
+      </c>
+      <c r="B323" t="s">
         <v>490</v>
       </c>
-      <c r="B323" t="s">
-        <v>491</v>
-      </c>
       <c r="C323" t="s">
+        <v>501</v>
+      </c>
+      <c r="D323" t="s">
         <v>502</v>
       </c>
-      <c r="D323" t="s">
-        <v>503</v>
-      </c>
       <c r="E323" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F323" s="10">
         <v>2863</v>
@@ -12645,16 +12671,16 @@
     </row>
     <row r="324" spans="1:7">
       <c r="A324" t="s">
+        <v>489</v>
+      </c>
+      <c r="B324" t="s">
         <v>490</v>
       </c>
-      <c r="B324" t="s">
-        <v>491</v>
-      </c>
       <c r="C324" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D324" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F324" s="10">
         <v>463698</v>
@@ -12665,16 +12691,16 @@
     </row>
     <row r="325" spans="1:7">
       <c r="A325" t="s">
+        <v>489</v>
+      </c>
+      <c r="B325" t="s">
         <v>490</v>
       </c>
-      <c r="B325" t="s">
-        <v>491</v>
-      </c>
       <c r="C325" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D325" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F325" s="10">
         <v>78662</v>
@@ -12709,7 +12735,7 @@
     </row>
     <row r="332" spans="1:7">
       <c r="A332" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F332" s="1">
         <f>365800000-SUM(F2:F331)</f>
@@ -12876,6 +12902,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>